<commit_message>
27-12-2017 : EmpMast Import removed MedCheckFlg and PoliceVerificationFlg
</commit_message>
<xml_diff>
--- a/upload_template/EmpMaster_Upload.xlsx
+++ b/upload_template/EmpMaster_Upload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anand\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>OTFLG</t>
-  </si>
-  <si>
-    <t>MedChkFlg</t>
   </si>
   <si>
     <t>PoliceVeriFlg</t>
@@ -603,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,22 +620,20 @@
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" customWidth="1"/>
-    <col min="27" max="27" width="11" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.42578125" customWidth="1"/>
-    <col min="31" max="31" width="16" style="1" customWidth="1"/>
-    <col min="32" max="32" width="27" style="1" customWidth="1"/>
-    <col min="33" max="33" width="28.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="25" max="25" width="11" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" customWidth="1"/>
+    <col min="29" max="29" width="16" style="1" customWidth="1"/>
+    <col min="30" max="30" width="27" style="1" customWidth="1"/>
+    <col min="31" max="31" width="28.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -661,7 +656,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>9</v>
@@ -670,7 +665,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>6</v>
@@ -681,151 +676,139 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="O1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="AB1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="AE1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9999999</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="S2" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="T2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="W2" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="X2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -846,22 +829,22 @@
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
@@ -890,16 +873,16 @@
         <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S10" t="s">
         <v>9</v>
       </c>
       <c r="T10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10" t="s">
         <v>51</v>
-      </c>
-      <c r="U10" t="s">
-        <v>52</v>
       </c>
       <c r="V10" t="s">
         <v>6</v>
@@ -911,34 +894,34 @@
         <v>13</v>
       </c>
       <c r="Y10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD10" t="s">
         <v>53</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AE10" t="s">
         <v>15</v>
       </c>
-      <c r="AA10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>16</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AG10" t="s">
         <v>17</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AH10" t="s">
         <v>18</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>19</v>
       </c>
       <c r="AI10" t="s">
         <v>7</v>
@@ -947,22 +930,22 @@
         <v>8</v>
       </c>
       <c r="AK10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AL10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM10" t="s">
         <v>55</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AN10" t="s">
         <v>56</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
         <v>57</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>58</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
@@ -997,7 +980,7 @@
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.25">
@@ -1007,12 +990,12 @@
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.25">
@@ -1032,52 +1015,52 @@
     </row>
     <row r="24" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.25">
@@ -1092,32 +1075,32 @@
     </row>
     <row r="36" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
05-03-2018 : Employee Master->include Employee Basic ->For Link with New ContractPayroll (BasicData , Import Employee), LeaveEntry Sorting Leave Details
</commit_message>
<xml_diff>
--- a/upload_template/EmpMaster_Upload.xlsx
+++ b/upload_template/EmpMaster_Upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -206,6 +206,21 @@
   </si>
   <si>
     <t>PACEHCEM01</t>
+  </si>
+  <si>
+    <t>BASIC</t>
+  </si>
+  <si>
+    <t>CONT</t>
+  </si>
+  <si>
+    <t>NRG</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2018-03-31</t>
   </si>
 </sst>
 </file>
@@ -600,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +648,7 @@
     <col min="31" max="31" width="28.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -727,8 +742,11 @@
       <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9999999</v>
       </c>
@@ -809,6 +827,104 @@
       </c>
       <c r="AC2" s="6" t="s">
         <v>44</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9999999</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
18-08-2018 : new process in scheduler ->Block/UnBlock
</commit_message>
<xml_diff>
--- a/upload_template/EmpMaster_Upload.xlsx
+++ b/upload_template/EmpMaster_Upload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance\upload_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance-NKP\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -217,16 +217,16 @@
     <t>NRG</t>
   </si>
   <si>
-    <t>2018-01-01</t>
-  </si>
-  <si>
-    <t>2018-03-31</t>
+    <t>SPLALL</t>
+  </si>
+  <si>
+    <t>BAALL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,8 +315,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -615,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +676,7 @@
     <col min="31" max="31" width="28.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -745,8 +773,14 @@
       <c r="AF1" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9999999</v>
       </c>
@@ -831,15 +865,21 @@
       <c r="AF2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9999999</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
@@ -854,10 +894,10 @@
       <c r="G3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>49</v>
       </c>
       <c r="J3" t="s">
@@ -878,53 +918,53 @@
       <c r="O3" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" t="s">
         <v>40</v>
       </c>
       <c r="Q3" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" t="s">
         <v>42</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" t="s">
         <v>32</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" t="s">
         <v>32</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AB3" t="s">
         <v>61</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AC3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="AF3">
         <v>320</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>